<commit_message>
Ajout 003MET + amelioration
</commit_message>
<xml_diff>
--- a/TNR_JDD/AD/JDD.AD.SEC.xlsx
+++ b/TNR_JDD/AD/JDD.AD.SEC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="10272" windowHeight="7644" tabRatio="395" activeTab="2"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="19056" windowHeight="3144" tabRatio="395" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -138,21 +138,6 @@
     <t>button_Connexion</t>
   </si>
   <si>
-    <t>//div[@id='desks']</t>
-  </si>
-  <si>
-    <t>div_Desk</t>
-  </si>
-  <si>
-    <t>//frame[@id='main']</t>
-  </si>
-  <si>
-    <t>frame_Main</t>
-  </si>
-  <si>
-    <t>il faut switcher sur frame_Main avant de tester le div_desk</t>
-  </si>
-  <si>
     <t>icon_Logout</t>
   </si>
   <si>
@@ -165,9 +150,6 @@
     <t>002</t>
   </si>
   <si>
-    <t>ALL</t>
-  </si>
-  <si>
     <t>LOCATOR</t>
   </si>
   <si>
@@ -175,6 +157,15 @@
   </si>
   <si>
     <t>wj7J4o1bGMA=</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>frame_Main</t>
+  </si>
+  <si>
+    <t>//frame[@id='main']</t>
   </si>
 </sst>
 </file>
@@ -389,7 +380,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -465,6 +456,8 @@
     <xf numFmtId="0" fontId="14" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2772,7 +2765,7 @@
   </sheetPr>
   <dimension ref="A1:C981"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -2794,7 +2787,7 @@
     </row>
     <row r="2" spans="1:3" ht="12" customHeight="1">
       <c r="A2" s="28" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>18</v>
@@ -2815,10 +2808,10 @@
         <v>21</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1">
@@ -5787,7 +5780,7 @@
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="28" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>18</v>
@@ -5805,7 +5798,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="25" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
@@ -8752,10 +8745,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -8764,7 +8757,7 @@
     <col min="3" max="3" width="86.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="18" t="s">
         <v>19</v>
       </c>
@@ -8775,7 +8768,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" s="19" t="s">
         <v>7</v>
       </c>
@@ -8786,7 +8779,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -8797,40 +8790,26 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="15" t="s">
-        <v>37</v>
+    <row r="4" spans="1:3">
+      <c r="A4" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>28</v>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="31" t="s">
+        <v>35</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="19" t="s">
+      <c r="B5" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>34</v>
+      <c r="C5" s="32" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add AD.SEC.001.FON.99 Ouvrir session OU reconnection pour moi :-)
</commit_message>
<xml_diff>
--- a/TNR_JDD/AD/JDD.AD.SEC.xlsx
+++ b/TNR_JDD/AD/JDD.AD.SEC.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>//span[@class='error']</t>
+  </si>
+  <si>
+    <t>AD.SEC.001.FON.99</t>
   </si>
 </sst>
 </file>
@@ -2935,7 +2938,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -3164,7 +3167,37 @@
       <c r="K9" s="28"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A10" s="11"/>
+      <c r="A10" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="28"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="11"/>

</xml_diff>